<commit_message>
chapter 5 example 5
</commit_message>
<xml_diff>
--- a/src/Chapter-5/03/部分信息/1.xlsx
+++ b/src/Chapter-5/03/部分信息/1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MGF\Documents\GitHub\TianXiaPy\PyExcel\src\Chapter-5\03\部分信息\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA367AAB-038D-440D-BC53-8E7CCFBEFFDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE33B3F-A4F9-4D6E-B45D-25D8AA29BBC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="1500" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="采购" sheetId="1" r:id="rId1"/>

</xml_diff>